<commit_message>
Funciona TODO! con date
</commit_message>
<xml_diff>
--- a/xls/personas.xlsx
+++ b/xls/personas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Personas</t>
   </si>
@@ -57,6 +57,27 @@
   </si>
   <si>
     <t>sexo,char</t>
+  </si>
+  <si>
+    <t>fecha,date</t>
+  </si>
+  <si>
+    <t>1991-12-12</t>
+  </si>
+  <si>
+    <t>1992-05-05</t>
+  </si>
+  <si>
+    <t>1993-04-03</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>Perezz</t>
+  </si>
+  <si>
+    <t>1993-02-03</t>
   </si>
 </sst>
 </file>
@@ -92,8 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,20 +393,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A7" sqref="A7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -397,8 +419,11 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -411,8 +436,11 @@
       <c r="D3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -425,8 +453,11 @@
       <c r="D4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -438,6 +469,43 @@
       </c>
       <c r="D5" t="s">
         <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>414</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>414</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>